<commit_message>
Added mothur join and qiime join
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/micans_v6_exp1/metadata.xlsx
+++ b/metadata/excel/projects/micans_v6_exp1/metadata.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="3020" windowWidth="50060" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="4620" windowWidth="50060" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_exp1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="296">
   <si>
     <t>Country</t>
   </si>
@@ -999,13 +999,13 @@
     <t>967F</t>
   </si>
   <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCTTTCCCTACACGACGCTCTTCCGATCT</t>
-  </si>
-  <si>
-    <t>CAAGCAGAAGACGGCATACGAGATCGTGATGTGACTGGAGTTCAGACGTGTGCTCTTCCGATCTCGACRRCCATGCA</t>
-  </si>
-  <si>
     <t>Short V6 primers</t>
+  </si>
+  <si>
+    <t>NNNNGAGACCTAACCGANGAACCTYACC</t>
+  </si>
+  <si>
+    <t>CNACGCGAAGAACCTTANC</t>
   </si>
 </sst>
 </file>
@@ -1620,9 +1620,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1641,6 +1638,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1928,7 +1928,7 @@
     <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="5">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1957,208 +1957,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2521,10 +2319,10 @@
   </sheetPr>
   <dimension ref="A1:BY69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <selection pane="bottomLeft" activeCell="AP44" sqref="AP44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2542,8 +2340,8 @@
     <col min="11" max="11" width="11.5" customWidth="1"/>
     <col min="12" max="12" width="10.33203125" style="39" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" style="39" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" style="59" customWidth="1"/>
-    <col min="15" max="15" width="14" style="62" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" style="58" customWidth="1"/>
+    <col min="15" max="15" width="14" style="61" customWidth="1"/>
     <col min="16" max="17" width="16.83203125" customWidth="1"/>
     <col min="18" max="18" width="11.5" customWidth="1"/>
     <col min="19" max="19" width="44.33203125" style="20" customWidth="1"/>
@@ -2566,9 +2364,9 @@
     <col min="36" max="36" width="10.33203125" customWidth="1"/>
     <col min="37" max="37" width="11.5" customWidth="1"/>
     <col min="38" max="38" width="19.6640625" customWidth="1"/>
-    <col min="39" max="39" width="12.83203125" style="63" customWidth="1"/>
+    <col min="39" max="39" width="12.83203125" style="62" customWidth="1"/>
     <col min="40" max="40" width="32.83203125" style="1" customWidth="1"/>
-    <col min="41" max="41" width="13" style="63" customWidth="1"/>
+    <col min="41" max="41" width="13" style="62" customWidth="1"/>
     <col min="42" max="42" width="35.6640625" style="1" customWidth="1"/>
     <col min="43" max="43" width="10.1640625" customWidth="1"/>
     <col min="44" max="44" width="12.5" customWidth="1"/>
@@ -2619,8 +2417,8 @@
       <c r="J1" s="38"/>
       <c r="L1" s="37"/>
       <c r="M1" s="38"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="60"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="59"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="8"/>
       <c r="S1" s="21"/>
@@ -2654,24 +2452,24 @@
       <c r="AX1" s="5"/>
       <c r="AY1" s="5"/>
       <c r="AZ1" s="12"/>
-      <c r="BB1" s="55" t="s">
+      <c r="BB1" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="BC1" s="55"/>
-      <c r="BD1" s="55"/>
-      <c r="BE1" s="55"/>
-      <c r="BG1" s="55" t="s">
+      <c r="BC1" s="63"/>
+      <c r="BD1" s="63"/>
+      <c r="BE1" s="63"/>
+      <c r="BG1" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="BH1" s="55"/>
-      <c r="BI1" s="55"/>
-      <c r="BJ1" s="55"/>
-      <c r="BK1" s="55"/>
-      <c r="BL1" s="55"/>
-      <c r="BN1" s="55" t="s">
+      <c r="BH1" s="63"/>
+      <c r="BI1" s="63"/>
+      <c r="BJ1" s="63"/>
+      <c r="BK1" s="63"/>
+      <c r="BL1" s="63"/>
+      <c r="BN1" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="BO1" s="55"/>
+      <c r="BO1" s="63"/>
       <c r="BQ1" s="10" t="s">
         <v>157</v>
       </c>
@@ -2719,10 +2517,10 @@
       <c r="M2" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="N2" s="57" t="s">
+      <c r="N2" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="57" t="s">
+      <c r="O2" s="56" t="s">
         <v>58</v>
       </c>
       <c r="P2" s="41" t="s">
@@ -2927,10 +2725,10 @@
       <c r="M3" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="N3" s="58">
+      <c r="N3" s="57">
         <v>1541441</v>
       </c>
-      <c r="O3" s="61">
+      <c r="O3" s="60">
         <v>1541441</v>
       </c>
       <c r="P3" s="31" t="s">
@@ -2974,19 +2772,19 @@
         <v>49</v>
       </c>
       <c r="AL3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM3" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO3" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP3" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM3" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO3" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ3" t="s">
         <v>49</v>
@@ -3065,10 +2863,10 @@
       <c r="M4" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="N4" s="58">
+      <c r="N4" s="57">
         <v>1513804</v>
       </c>
-      <c r="O4" s="61">
+      <c r="O4" s="60">
         <v>1513804</v>
       </c>
       <c r="P4" s="31" t="s">
@@ -3112,19 +2910,19 @@
         <v>49</v>
       </c>
       <c r="AL4" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM4" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO4" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP4" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM4" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO4" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ4" t="s">
         <v>49</v>
@@ -3203,10 +3001,10 @@
       <c r="M5" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="N5" s="58">
+      <c r="N5" s="57">
         <v>1563302</v>
       </c>
-      <c r="O5" s="61">
+      <c r="O5" s="60">
         <v>1563302</v>
       </c>
       <c r="P5" s="31" t="s">
@@ -3250,19 +3048,19 @@
         <v>49</v>
       </c>
       <c r="AL5" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM5" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO5" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP5" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM5" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN5" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO5" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ5" t="s">
         <v>49</v>
@@ -3341,10 +3139,10 @@
       <c r="M6" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="N6" s="58">
+      <c r="N6" s="57">
         <v>1565845</v>
       </c>
-      <c r="O6" s="61">
+      <c r="O6" s="60">
         <v>1565845</v>
       </c>
       <c r="P6" s="32" t="s">
@@ -3388,19 +3186,19 @@
         <v>49</v>
       </c>
       <c r="AL6" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM6" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO6" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP6" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM6" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO6" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ6" t="s">
         <v>49</v>
@@ -3479,10 +3277,10 @@
       <c r="M7" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="N7" s="58">
+      <c r="N7" s="57">
         <v>677372</v>
       </c>
-      <c r="O7" s="61">
+      <c r="O7" s="60">
         <v>677372</v>
       </c>
       <c r="P7" s="31" t="s">
@@ -3526,19 +3324,19 @@
         <v>49</v>
       </c>
       <c r="AL7" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM7" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO7" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP7" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM7" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO7" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP7" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ7" t="s">
         <v>49</v>
@@ -3617,10 +3415,10 @@
       <c r="M8" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="N8" s="58">
+      <c r="N8" s="57">
         <v>663201</v>
       </c>
-      <c r="O8" s="61">
+      <c r="O8" s="60">
         <v>663201</v>
       </c>
       <c r="P8" s="31" t="s">
@@ -3664,19 +3462,19 @@
         <v>49</v>
       </c>
       <c r="AL8" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM8" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO8" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP8" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM8" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN8" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO8" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP8" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ8" t="s">
         <v>49</v>
@@ -3755,10 +3553,10 @@
       <c r="M9" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="N9" s="58">
+      <c r="N9" s="57">
         <v>686948</v>
       </c>
-      <c r="O9" s="61">
+      <c r="O9" s="60">
         <v>686948</v>
       </c>
       <c r="P9" s="31" t="s">
@@ -3802,19 +3600,19 @@
         <v>49</v>
       </c>
       <c r="AL9" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM9" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO9" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP9" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM9" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN9" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO9" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP9" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ9" t="s">
         <v>49</v>
@@ -3893,10 +3691,10 @@
       <c r="M10" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="N10" s="58">
+      <c r="N10" s="57">
         <v>686723</v>
       </c>
-      <c r="O10" s="61">
+      <c r="O10" s="60">
         <v>686723</v>
       </c>
       <c r="P10" s="31" t="s">
@@ -3940,19 +3738,19 @@
         <v>49</v>
       </c>
       <c r="AL10" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM10" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO10" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP10" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM10" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN10" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO10" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP10" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ10" t="s">
         <v>49</v>
@@ -4031,10 +3829,10 @@
       <c r="M11" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="N11" s="58">
+      <c r="N11" s="57">
         <v>1539394</v>
       </c>
-      <c r="O11" s="61">
+      <c r="O11" s="60">
         <v>1539394</v>
       </c>
       <c r="P11" s="31" t="s">
@@ -4078,19 +3876,19 @@
         <v>49</v>
       </c>
       <c r="AL11" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM11" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO11" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP11" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM11" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN11" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO11" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP11" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ11" t="s">
         <v>49</v>
@@ -4169,10 +3967,10 @@
       <c r="M12" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="N12" s="58">
+      <c r="N12" s="57">
         <v>1510757</v>
       </c>
-      <c r="O12" s="61">
+      <c r="O12" s="60">
         <v>1510757</v>
       </c>
       <c r="P12" s="31" t="s">
@@ -4216,19 +4014,19 @@
         <v>49</v>
       </c>
       <c r="AL12" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM12" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO12" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP12" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM12" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN12" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO12" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP12" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ12" t="s">
         <v>49</v>
@@ -4307,10 +4105,10 @@
       <c r="M13" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="N13" s="58">
+      <c r="N13" s="57">
         <v>1562525</v>
       </c>
-      <c r="O13" s="61">
+      <c r="O13" s="60">
         <v>1562525</v>
       </c>
       <c r="P13" s="31" t="s">
@@ -4354,19 +4152,19 @@
         <v>49</v>
       </c>
       <c r="AL13" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM13" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN13" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO13" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP13" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM13" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN13" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO13" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP13" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ13" t="s">
         <v>49</v>
@@ -4445,10 +4243,10 @@
       <c r="M14" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="N14" s="58">
+      <c r="N14" s="57">
         <v>1560693</v>
       </c>
-      <c r="O14" s="61">
+      <c r="O14" s="60">
         <v>1560693</v>
       </c>
       <c r="P14" s="31" t="s">
@@ -4492,19 +4290,19 @@
         <v>49</v>
       </c>
       <c r="AL14" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM14" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN14" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO14" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP14" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM14" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN14" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO14" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP14" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ14" t="s">
         <v>49</v>
@@ -4583,10 +4381,10 @@
       <c r="M15" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="N15" s="58">
+      <c r="N15" s="57">
         <v>1033095</v>
       </c>
-      <c r="O15" s="61">
+      <c r="O15" s="60">
         <v>1033095</v>
       </c>
       <c r="P15" s="31" t="s">
@@ -4630,19 +4428,19 @@
         <v>49</v>
       </c>
       <c r="AL15" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM15" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN15" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO15" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP15" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM15" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN15" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO15" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP15" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ15" t="s">
         <v>49</v>
@@ -4721,10 +4519,10 @@
       <c r="M16" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="N16" s="58">
+      <c r="N16" s="57">
         <v>1012051</v>
       </c>
-      <c r="O16" s="61">
+      <c r="O16" s="60">
         <v>1012051</v>
       </c>
       <c r="P16" s="31" t="s">
@@ -4768,19 +4566,19 @@
         <v>49</v>
       </c>
       <c r="AL16" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM16" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN16" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO16" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP16" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM16" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN16" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO16" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP16" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ16" t="s">
         <v>49</v>
@@ -4859,10 +4657,10 @@
       <c r="M17" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="N17" s="58">
+      <c r="N17" s="57">
         <v>1045841</v>
       </c>
-      <c r="O17" s="61">
+      <c r="O17" s="60">
         <v>1045841</v>
       </c>
       <c r="P17" s="32" t="s">
@@ -4906,19 +4704,19 @@
         <v>49</v>
       </c>
       <c r="AL17" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM17" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN17" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO17" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP17" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM17" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN17" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO17" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP17" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ17" t="s">
         <v>49</v>
@@ -4997,10 +4795,10 @@
       <c r="M18" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="N18" s="58">
+      <c r="N18" s="57">
         <v>1045591</v>
       </c>
-      <c r="O18" s="61">
+      <c r="O18" s="60">
         <v>1045591</v>
       </c>
       <c r="P18" s="31" t="s">
@@ -5044,19 +4842,19 @@
         <v>49</v>
       </c>
       <c r="AL18" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM18" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN18" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO18" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP18" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM18" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN18" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO18" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP18" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ18" t="s">
         <v>49</v>
@@ -5135,10 +4933,10 @@
       <c r="M19" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="N19" s="58">
+      <c r="N19" s="57">
         <v>911612</v>
       </c>
-      <c r="O19" s="61">
+      <c r="O19" s="60">
         <v>911612</v>
       </c>
       <c r="P19" s="31" t="s">
@@ -5182,19 +4980,19 @@
         <v>49</v>
       </c>
       <c r="AL19" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM19" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN19" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO19" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP19" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM19" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN19" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO19" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP19" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ19" t="s">
         <v>49</v>
@@ -5273,10 +5071,10 @@
       <c r="M20" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="N20" s="58">
+      <c r="N20" s="57">
         <v>890088</v>
       </c>
-      <c r="O20" s="61">
+      <c r="O20" s="60">
         <v>890088</v>
       </c>
       <c r="P20" s="31" t="s">
@@ -5320,19 +5118,19 @@
         <v>49</v>
       </c>
       <c r="AL20" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM20" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN20" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO20" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP20" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM20" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN20" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO20" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP20" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ20" t="s">
         <v>49</v>
@@ -5411,10 +5209,10 @@
       <c r="M21" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="N21" s="58">
+      <c r="N21" s="57">
         <v>922452</v>
       </c>
-      <c r="O21" s="61">
+      <c r="O21" s="60">
         <v>922452</v>
       </c>
       <c r="P21" s="31" t="s">
@@ -5458,19 +5256,19 @@
         <v>49</v>
       </c>
       <c r="AL21" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM21" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN21" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO21" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP21" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM21" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN21" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO21" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP21" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ21" t="s">
         <v>49</v>
@@ -5549,10 +5347,10 @@
       <c r="M22" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="N22" s="58">
+      <c r="N22" s="57">
         <v>920466</v>
       </c>
-      <c r="O22" s="61">
+      <c r="O22" s="60">
         <v>920466</v>
       </c>
       <c r="P22" s="31" t="s">
@@ -5596,19 +5394,19 @@
         <v>49</v>
       </c>
       <c r="AL22" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM22" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN22" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO22" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP22" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM22" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN22" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO22" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP22" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ22" t="s">
         <v>49</v>
@@ -5687,10 +5485,10 @@
       <c r="M23" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="N23" s="58">
+      <c r="N23" s="57">
         <v>3067661</v>
       </c>
-      <c r="O23" s="61">
+      <c r="O23" s="60">
         <v>3067661</v>
       </c>
       <c r="P23" s="31" t="s">
@@ -5734,19 +5532,19 @@
         <v>49</v>
       </c>
       <c r="AL23" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM23" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN23" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO23" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP23" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM23" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN23" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO23" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP23" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ23" t="s">
         <v>49</v>
@@ -5825,10 +5623,10 @@
       <c r="M24" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="N24" s="58">
+      <c r="N24" s="57">
         <v>3009815</v>
       </c>
-      <c r="O24" s="61">
+      <c r="O24" s="60">
         <v>3009815</v>
       </c>
       <c r="P24" s="31" t="s">
@@ -5872,19 +5670,19 @@
         <v>49</v>
       </c>
       <c r="AL24" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM24" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN24" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO24" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP24" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM24" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN24" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO24" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP24" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ24" t="s">
         <v>49</v>
@@ -5963,10 +5761,10 @@
       <c r="M25" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="N25" s="58">
+      <c r="N25" s="57">
         <v>3108035</v>
       </c>
-      <c r="O25" s="61">
+      <c r="O25" s="60">
         <v>3108035</v>
       </c>
       <c r="P25" s="31" t="s">
@@ -6010,19 +5808,19 @@
         <v>49</v>
       </c>
       <c r="AL25" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM25" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN25" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO25" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP25" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM25" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN25" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO25" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP25" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ25" t="s">
         <v>49</v>
@@ -6101,10 +5899,10 @@
       <c r="M26" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="N26" s="58">
+      <c r="N26" s="57">
         <v>3114749</v>
       </c>
-      <c r="O26" s="61">
+      <c r="O26" s="60">
         <v>3114749</v>
       </c>
       <c r="P26" s="31" t="s">
@@ -6148,19 +5946,19 @@
         <v>49</v>
       </c>
       <c r="AL26" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM26" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN26" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO26" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP26" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM26" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN26" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO26" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP26" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ26" t="s">
         <v>49</v>
@@ -6239,10 +6037,10 @@
       <c r="M27" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="N27" s="58">
+      <c r="N27" s="57">
         <v>2634261</v>
       </c>
-      <c r="O27" s="61">
+      <c r="O27" s="60">
         <v>2634261</v>
       </c>
       <c r="P27" s="31" t="s">
@@ -6286,19 +6084,19 @@
         <v>49</v>
       </c>
       <c r="AL27" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM27" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN27" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO27" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP27" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM27" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN27" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO27" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP27" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ27" t="s">
         <v>49</v>
@@ -6377,10 +6175,10 @@
       <c r="M28" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="N28" s="58">
+      <c r="N28" s="57">
         <v>2572925</v>
       </c>
-      <c r="O28" s="61">
+      <c r="O28" s="60">
         <v>2572925</v>
       </c>
       <c r="P28" s="31" t="s">
@@ -6424,19 +6222,19 @@
         <v>49</v>
       </c>
       <c r="AL28" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM28" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN28" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO28" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP28" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM28" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN28" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO28" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP28" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ28" t="s">
         <v>49</v>
@@ -6515,10 +6313,10 @@
       <c r="M29" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="N29" s="58">
+      <c r="N29" s="57">
         <v>2670122</v>
       </c>
-      <c r="O29" s="61">
+      <c r="O29" s="60">
         <v>2670122</v>
       </c>
       <c r="P29" s="31" t="s">
@@ -6562,19 +6360,19 @@
         <v>49</v>
       </c>
       <c r="AL29" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM29" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN29" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO29" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP29" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM29" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN29" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO29" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP29" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ29" t="s">
         <v>49</v>
@@ -6653,10 +6451,10 @@
       <c r="M30" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="N30" s="58">
+      <c r="N30" s="57">
         <v>2666598</v>
       </c>
-      <c r="O30" s="61">
+      <c r="O30" s="60">
         <v>2666598</v>
       </c>
       <c r="P30" s="31" t="s">
@@ -6700,19 +6498,19 @@
         <v>49</v>
       </c>
       <c r="AL30" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM30" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN30" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO30" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP30" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM30" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN30" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO30" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP30" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ30" t="s">
         <v>49</v>
@@ -6791,10 +6589,10 @@
       <c r="M31" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="N31" s="58">
+      <c r="N31" s="57">
         <v>1678404</v>
       </c>
-      <c r="O31" s="61">
+      <c r="O31" s="60">
         <v>1678404</v>
       </c>
       <c r="P31" s="31" t="s">
@@ -6838,19 +6636,19 @@
         <v>49</v>
       </c>
       <c r="AL31" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM31" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN31" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO31" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP31" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM31" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN31" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO31" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP31" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ31" t="s">
         <v>49</v>
@@ -6929,10 +6727,10 @@
       <c r="M32" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="N32" s="58">
+      <c r="N32" s="57">
         <v>1640506</v>
       </c>
-      <c r="O32" s="61">
+      <c r="O32" s="60">
         <v>1640506</v>
       </c>
       <c r="P32" s="31" t="s">
@@ -6976,19 +6774,19 @@
         <v>49</v>
       </c>
       <c r="AL32" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM32" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN32" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO32" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP32" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM32" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN32" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO32" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP32" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ32" t="s">
         <v>49</v>
@@ -7067,10 +6865,10 @@
       <c r="M33" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="N33" s="58">
+      <c r="N33" s="57">
         <v>1702829</v>
       </c>
-      <c r="O33" s="61">
+      <c r="O33" s="60">
         <v>1702829</v>
       </c>
       <c r="P33" s="32" t="s">
@@ -7114,19 +6912,19 @@
         <v>49</v>
       </c>
       <c r="AL33" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM33" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN33" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO33" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP33" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM33" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN33" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO33" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP33" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ33" t="s">
         <v>49</v>
@@ -7205,10 +7003,10 @@
       <c r="M34" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="N34" s="58">
+      <c r="N34" s="57">
         <v>1699601</v>
       </c>
-      <c r="O34" s="61">
+      <c r="O34" s="60">
         <v>1699601</v>
       </c>
       <c r="P34" s="31" t="s">
@@ -7252,19 +7050,19 @@
         <v>49</v>
       </c>
       <c r="AL34" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM34" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN34" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO34" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP34" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM34" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN34" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO34" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP34" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ34" t="s">
         <v>49</v>
@@ -7343,10 +7141,10 @@
       <c r="M35" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="N35" s="58">
+      <c r="N35" s="57">
         <v>1677838</v>
       </c>
-      <c r="O35" s="61">
+      <c r="O35" s="60">
         <v>1677838</v>
       </c>
       <c r="P35" s="31" t="s">
@@ -7390,19 +7188,19 @@
         <v>49</v>
       </c>
       <c r="AL35" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM35" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN35" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO35" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP35" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM35" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN35" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO35" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP35" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ35" t="s">
         <v>49</v>
@@ -7481,10 +7279,10 @@
       <c r="M36" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="N36" s="58">
+      <c r="N36" s="57">
         <v>1637501</v>
       </c>
-      <c r="O36" s="61">
+      <c r="O36" s="60">
         <v>1637501</v>
       </c>
       <c r="P36" s="31" t="s">
@@ -7528,19 +7326,19 @@
         <v>49</v>
       </c>
       <c r="AL36" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM36" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN36" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO36" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP36" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="AM36" s="63" t="s">
-        <v>292</v>
-      </c>
-      <c r="AN36" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AO36" s="63" t="s">
-        <v>291</v>
-      </c>
-      <c r="AP36" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AQ36" t="s">
         <v>49</v>
@@ -7620,10 +7418,10 @@
       <c r="M37" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="N37" s="59">
+      <c r="N37" s="58">
         <v>1699067</v>
       </c>
-      <c r="O37" s="62">
+      <c r="O37" s="61">
         <v>1699067</v>
       </c>
       <c r="P37" t="s">
@@ -7662,9 +7460,54 @@
       <c r="AF37"/>
       <c r="AG37"/>
       <c r="AI37"/>
-      <c r="AJ37" s="15"/>
-      <c r="AN37"/>
-      <c r="AP37"/>
+      <c r="AJ37" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM37" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN37" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO37" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP37" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="AQ37" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU37" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW37" t="s">
+        <v>290</v>
+      </c>
+      <c r="AY37">
+        <v>111</v>
+      </c>
+      <c r="AZ37">
+        <v>111</v>
+      </c>
       <c r="BH37"/>
       <c r="BI37"/>
       <c r="BJ37"/>
@@ -7715,10 +7558,10 @@
       <c r="M38" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="N38" s="59">
+      <c r="N38" s="58">
         <v>1691153</v>
       </c>
-      <c r="O38" s="62">
+      <c r="O38" s="61">
         <v>1691153</v>
       </c>
       <c r="P38" t="s">
@@ -7757,9 +7600,54 @@
       <c r="AF38"/>
       <c r="AG38"/>
       <c r="AI38"/>
-      <c r="AJ38" s="15"/>
-      <c r="AN38"/>
-      <c r="AP38"/>
+      <c r="AJ38" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM38" s="62" t="s">
+        <v>292</v>
+      </c>
+      <c r="AN38" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO38" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP38" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="AQ38" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS38" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT38" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU38" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV38" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW38" t="s">
+        <v>290</v>
+      </c>
+      <c r="AY38">
+        <v>111</v>
+      </c>
+      <c r="AZ38">
+        <v>111</v>
+      </c>
       <c r="BH38"/>
       <c r="BI38"/>
       <c r="BJ38"/>
@@ -7931,9 +7819,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -7951,24 +7849,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>